<commit_message>
Adding first set suite and test cases
</commit_message>
<xml_diff>
--- a/TestAutomation/src/main/java/testdata/TestData.xlsx
+++ b/TestAutomation/src/main/java/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11760" windowHeight="4905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11070" windowHeight="2970" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G14"/>
+  <oleSize ref="A1:K8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>10001_verifythatUserCanAbleToLoginUsingValidCredentials</t>
   </si>
@@ -65,6 +65,90 @@
   </si>
   <si>
     <t>browser Name</t>
+  </si>
+  <si>
+    <t>Serial No</t>
+  </si>
+  <si>
+    <t>Test Suite</t>
+  </si>
+  <si>
+    <t>Testcase</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>TestcaseId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_10001_verify that user can able to perform following actions:Selecting an item,registration, and ordering an item </t>
+  </si>
+  <si>
+    <t>test_10002_verify thet user can able to click add to cart button and confirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_10003_verify that user can able to perform mouse hower on cart drop down confirm the details and click on checkout button </t>
+  </si>
+  <si>
+    <t>test_10004_verify that user can able to click on close button present in drop down to cancel the order</t>
+  </si>
+  <si>
+    <t>test_10005_verify that user can able to cancel the checkout by clicking on delete button and confirm on shopping cart summary page</t>
+  </si>
+  <si>
+    <t>test_10006_verify that item image is present in the first column on shopping cart summary page</t>
+  </si>
+  <si>
+    <t>test_10007_verify that order details are present in the shopping cart summary page</t>
+  </si>
+  <si>
+    <t>test_10008_verify that five work flows like summary,sign in,Address,shipping and payment are available in shopping cart summary page</t>
+  </si>
+  <si>
+    <t>test_10010_verify that user can click on proceed checkout page from shopping cart summary page</t>
+  </si>
+  <si>
+    <t>test_10009_verify that user can able to increase and reduce the quantity from shopping cart summary page</t>
+  </si>
+  <si>
+    <t>As a Guest User:Checkout</t>
+  </si>
+  <si>
+    <t>test_10011_verify that order detail total is correct by adding quantity and reducing the quantity</t>
+  </si>
+  <si>
+    <t>test_10012_verify that user entered emailid is correct in authentication page</t>
+  </si>
+  <si>
+    <t>test_10013_verify that if user enters existing email id , application throwing error while registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_10014_verify that user can able to register new account </t>
+  </si>
+  <si>
+    <t>test_10015 _verify that user can able to register account</t>
+  </si>
+  <si>
+    <t>test_10016_verify that user address is correct</t>
+  </si>
+  <si>
+    <t>test_10017_verify that user can able to perform proceed checkout</t>
+  </si>
+  <si>
+    <t>test_10018_verify that user can able to confirm shipping by clicking terms and conditions and proceed check out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_10019_verify that user can able topay by pay by bank </t>
+  </si>
+  <si>
+    <t>test_10020_verify that user can able to pay by check</t>
+  </si>
+  <si>
+    <t>test_10021_verify that user can able to confirm the order and confirm</t>
   </si>
 </sst>
 </file>
@@ -141,13 +225,18 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,7 +535,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -504,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -554,12 +643,299 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="103.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="6" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10001</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1">
+        <v>10002</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1">
+        <v>10003</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1">
+        <v>10004</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1">
+        <v>10005</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="1">
+        <v>10006</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="1">
+        <v>10007</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="1">
+        <v>10008</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="1">
+        <v>10009</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="1">
+        <v>10010</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1">
+        <v>10011</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="1">
+        <v>10012</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="1">
+        <v>10013</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="1">
+        <v>10014</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="1">
+        <v>10015</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="1">
+        <v>10016</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="1">
+        <v>10017</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="1">
+        <v>10018</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="1">
+        <v>10019</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="1">
+        <v>10020</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="1">
+        <v>10021</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:B22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completion of First testcase
</commit_message>
<xml_diff>
--- a/TestAutomation/src/main/java/testdata/TestData.xlsx
+++ b/TestAutomation/src/main/java/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11070" windowHeight="4830" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12285" windowHeight="4830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:K8"/>
+  <oleSize ref="A1:D14"/>
 </workbook>
 </file>
 
@@ -148,7 +148,7 @@
     <t>test_10021_verify that user can able to confirm the order and confirm</t>
   </si>
   <si>
-    <t>test_10002_VerifyThetUserCanAbleToClickItem()</t>
+    <t>test_10002_VerifyThetUserCanAbleToClickQuickViewItemAndVerifyTheDetails()</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,7 +645,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>